<commit_message>
Made progress on preprocessing - ohe, ordinal, scaled, impute
</commit_message>
<xml_diff>
--- a/Preprocessing.xlsx
+++ b/Preprocessing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanjays/Desktop/Programming/Flatiron/Flat_Iron_Repo/dsc_project3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69FEA41-5B3F-A044-A708-958296660A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB94449-A6E1-DD43-B99C-1CC51CD9F2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1320" windowWidth="38400" windowHeight="21140" xr2:uid="{38B905FA-0969-5448-8058-A93E282E509C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{38B905FA-0969-5448-8058-A93E282E509C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -545,7 +545,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>